<commit_message>
dossier AVP SAO final
</commit_message>
<xml_diff>
--- a/7 - Recherche Entrées/1 - Subventions/2022-2023/AVP-SAO/DossierSubventionsUnipoly2223/Modele-Documents_comptables_Subvention-SAO-2023.xlsx
+++ b/7 - Recherche Entrées/1 - Subventions/2022-2023/AVP-SAO/DossierSubventionsUnipoly2223/Modele-Documents_comptables_Subvention-SAO-2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\Clara\Unipoly\UPSecretrariat\7 - Recherche Entrées\1 - Subventions\2022-2023\AVP-SAO\Dossier en cours\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\Clara\Unipoly\UPSecretrariat\7 - Recherche Entrées\1 - Subventions\2022-2023\AVP-SAO\DossierSubventionsUnipoly2223\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{EF5196EA-4D64-4817-B95B-3C34E5C21D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192B0CDD-E238-4574-8C6C-3DB528765EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,7 +196,6 @@
     <definedName name="Z_BFDCD700_5607_11D7_98B8_0001020B4F98_.wvu.Rows" localSheetId="0">'Profits et Pertes'!#REF!,'Profits et Pertes'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -925,16 +924,40 @@
   </si>
   <si>
     <r>
-      <t>Bilan au</t>
+      <t>Ecublens
+Estimation Bilan au</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 31 août </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>2023</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Bilan a</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> 31 août </t>
+      <t xml:space="preserve">u 31 août </t>
     </r>
     <r>
       <rPr>
@@ -945,30 +968,6 @@
       </rPr>
       <t xml:space="preserve">
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ecublens
-Estimation Bilan au </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">1 janvier </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>2023</t>
     </r>
   </si>
 </sst>
@@ -983,7 +982,7 @@
     <numFmt numFmtId="167" formatCode="_ * #,##0.00_)\ _C_H_F_ ;_ * \(#,##0.00\)\ _C_H_F_ ;_ * &quot;-&quot;??_)\ _C_H_F_ ;_ @_ "/>
     <numFmt numFmtId="168" formatCode="0.0\ "/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1133,14 +1132,28 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1525,10 +1538,13 @@
     <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1541,16 +1557,13 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1803,7 +1816,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="114" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="113"/>
@@ -1833,7 +1846,7 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="115" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="113"/>
@@ -1863,7 +1876,7 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="115"/>
+      <c r="A3" s="116"/>
       <c r="B3" s="113"/>
       <c r="C3" s="113"/>
       <c r="D3" s="113"/>
@@ -1891,7 +1904,7 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="117" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="113"/>
@@ -1921,7 +1934,7 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="118" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="113"/>
@@ -2035,7 +2048,7 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="118"/>
+      <c r="A9" s="112"/>
       <c r="B9" s="113"/>
       <c r="C9" s="113"/>
       <c r="D9" s="113"/>
@@ -30792,8 +30805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -30808,7 +30821,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="114" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="113"/>
@@ -30838,8 +30851,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="119" t="s">
-        <v>123</v>
+      <c r="A2" s="120" t="s">
+        <v>122</v>
       </c>
       <c r="B2" s="113"/>
       <c r="C2" s="113"/>
@@ -30868,7 +30881,7 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="119" t="s">
         <v>83</v>
       </c>
       <c r="B3" s="113"/>
@@ -30899,7 +30912,7 @@
     </row>
     <row r="4" spans="1:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="121" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B4" s="113"/>
       <c r="C4" s="113"/>
@@ -30928,7 +30941,7 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="114"/>
+      <c r="A5" s="115"/>
       <c r="B5" s="113"/>
       <c r="C5" s="113"/>
       <c r="D5" s="113"/>
@@ -59194,7 +59207,7 @@
     <mergeCell ref="A5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="49" orientation="landscape"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="49" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>